<commit_message>
Update Laporan Harian Scrummaster
</commit_message>
<xml_diff>
--- a/BACKLOG TKPPL.xlsx
+++ b/BACKLOG TKPPL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7155" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Scrummaster" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Penjelasan Tahapan Persiapan dan Sebelum memulai Proyek dengan Trello.</t>
   </si>
@@ -38,27 +38,6 @@
     <t>Product Backlog :</t>
   </si>
   <si>
-    <t>1. Penjelasan secara Umum : Apa itu Dota</t>
-  </si>
-  <si>
-    <t>2. Penjelasan secara Umum : Elemem pada Dota (Game Mode, Aktor, Item)</t>
-  </si>
-  <si>
-    <t>3. Penjelasan secara Umum : Game Mode Dota (Penjelasan, Beberapa Contoh)</t>
-  </si>
-  <si>
-    <t>4. Penjelasan secara Umum : "Aktor" yang ada pada Dota (Penjelasan untuk Creeps, Neutral Creeps, Tower, Ancient, Hero)</t>
-  </si>
-  <si>
-    <t>6. Penjelasan secara Umum : Aturan Bermain Dota</t>
-  </si>
-  <si>
-    <t>5. Penjelasan secara Umum : Effect Item pada Dota (Jenis dan Penjelasan, Beberapa Contoh)</t>
-  </si>
-  <si>
-    <t>7. Penjelasan secara Umum : Manfaat Bermain Dota</t>
-  </si>
-  <si>
     <t>8. Edit Fungsionalitas dan Tampilan Bespoke</t>
   </si>
   <si>
@@ -95,15 +74,6 @@
     <t>19. Warding : Penjelasan</t>
   </si>
   <si>
-    <t>Spint Backlog :</t>
-  </si>
-  <si>
-    <t>In Progress :</t>
-  </si>
-  <si>
-    <t>Done :</t>
-  </si>
-  <si>
     <t>Dikarenakan Backlog terlalu banyak, mohon cek penjelasan dibawah gambar agar dapat melihat isi dari semua backlog yang ada.</t>
   </si>
   <si>
@@ -168,6 +138,30 @@
   </si>
   <si>
     <t>21. Warding : Jenis-Jenis Strategi Warding</t>
+  </si>
+  <si>
+    <t>Done:</t>
+  </si>
+  <si>
+    <t>1. Penjelasan secara Umum : Apa itu Dota2</t>
+  </si>
+  <si>
+    <t>3. Penjelasan secara Umum : Game Mode Dota2 (Penjelasan, Beberapa Contoh)</t>
+  </si>
+  <si>
+    <t>4. Penjelasan secara Umum : "Aktor" yang ada pada Dota2 (Penjelasan untuk Creeps, Neutral Creeps, Tower, Ancient, Hero)</t>
+  </si>
+  <si>
+    <t>5. Penjelasan secara Umum : Effect Item pada Dota2 (Jenis dan Penjelasan, Beberapa Contoh)</t>
+  </si>
+  <si>
+    <t>6. Penjelasan secara Umum : Aturan Bermain Dota2</t>
+  </si>
+  <si>
+    <t>7. Penjelasan secara Umum : Manfaat Bermain Dota2</t>
+  </si>
+  <si>
+    <t>2. Penjelasan secara Umum : Elemen pada Dota2 (Game Mode, Aktor, Item)</t>
   </si>
 </sst>
 </file>
@@ -560,13 +554,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -712,57 +706,57 @@
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -778,7 +772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W83"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -930,7 +924,7 @@
     </row>
     <row r="10" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -943,156 +937,152 @@
         <v>1</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="83" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B83" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O83" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="B83" s="1"/>
+      <c r="O83" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Tambah Role : Carry
</commit_message>
<xml_diff>
--- a/BACKLOG TKPPL.xlsx
+++ b/BACKLOG TKPPL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7155" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7155" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Scrummaster" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="72">
   <si>
     <t>Penjelasan Tahapan Persiapan dan Sebelum memulai Proyek dengan Trello.</t>
   </si>
@@ -162,6 +162,90 @@
   </si>
   <si>
     <t>2. Penjelasan secara Umum : Elemen pada Dota2 (Game Mode, Aktor, Item)</t>
+  </si>
+  <si>
+    <t>Penjelasan Hasil Sprint Pertama dengan Trello.</t>
+  </si>
+  <si>
+    <t>1. Penjelasan secara Umum : Game Mode Dota2 (Penjelasan, Beberapa Contoh)</t>
+  </si>
+  <si>
+    <t>2. Penjelasan secara Umum : "Aktor" yang ada pada Dota2 (Penjelasan untuk Creeps, Neutral Creeps, Tower, Ancient, Hero)</t>
+  </si>
+  <si>
+    <t>3. Penjelasan secara Umum : Effect Item pada Dota2 (Jenis dan Penjelasan, Beberapa Contoh)</t>
+  </si>
+  <si>
+    <t>4. Penjelasan secara Umum : Aturan Bermain Dota2</t>
+  </si>
+  <si>
+    <t>5. Penjelasan secara Umum : Manfaat Bermain Dota2</t>
+  </si>
+  <si>
+    <t>6. Role : Disabler</t>
+  </si>
+  <si>
+    <t>7. Role : Lane Support</t>
+  </si>
+  <si>
+    <t>8. Role : Initiator</t>
+  </si>
+  <si>
+    <t>9. Role : Jungler</t>
+  </si>
+  <si>
+    <t>10. Role : Support</t>
+  </si>
+  <si>
+    <t>11. Role : Durable</t>
+  </si>
+  <si>
+    <t>12. Role : Nuker</t>
+  </si>
+  <si>
+    <t>13. Role : Pusher</t>
+  </si>
+  <si>
+    <t>14. Role : Escape</t>
+  </si>
+  <si>
+    <t>15. Warding : Manfaat Warding</t>
+  </si>
+  <si>
+    <t>16. Warding : Jenis-Jenis Strategi Warding</t>
+  </si>
+  <si>
+    <t>17. Warding : Pembagian Ward (Penjelasan untuk Observer &amp; Sentry)</t>
+  </si>
+  <si>
+    <t>18. Warding : Lokasi Ideal untuk Warding</t>
+  </si>
+  <si>
+    <t>19. Hero Guide Sniper : Item Build (Early, Mid, Late)</t>
+  </si>
+  <si>
+    <t>20. Hero Guide Sniper : Strategy (Early, Mid, Late)</t>
+  </si>
+  <si>
+    <t>21. Hero Guide Sniper : Best "Friends"</t>
+  </si>
+  <si>
+    <t>22. Hero Guide Sniper : Worst "Enemies"</t>
+  </si>
+  <si>
+    <t>3. Edit Fungsionalitas dan Tampilan Bespoke</t>
+  </si>
+  <si>
+    <t>4. Role : Carry</t>
+  </si>
+  <si>
+    <t>5. Warding : Penjelasan</t>
+  </si>
+  <si>
+    <t>6. Hero Guide Sniper : Penjelasan Singkat (Tipe, Skills)</t>
+  </si>
+  <si>
+    <t>Ket : Untuk Penjelasan secara Umum : Elemen pada Dota2 (Game Mode, Aktor, Item) yang harusnya digeser ke Done oleh Javentira Lienata digantikan oleh ScrumMaster Sprint 1 (William Limianto) karena berhalangan.</t>
   </si>
 </sst>
 </file>
@@ -278,6 +362,49 @@
         <a:xfrm>
           <a:off x="593910" y="2237974"/>
           <a:ext cx="13000007" cy="7304762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>47627</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>119059</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>588936</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>127797</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="666752" y="2690809"/>
+          <a:ext cx="12923809" cy="6295238"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -772,7 +899,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView topLeftCell="A44" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B52" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1096,13 +1225,320 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:W83"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+    </row>
+    <row r="10" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O52" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>45</v>
+      </c>
+      <c r="O53" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>46</v>
+      </c>
+      <c r="O54" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>47</v>
+      </c>
+      <c r="O55" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>48</v>
+      </c>
+      <c r="O56" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>49</v>
+      </c>
+      <c r="O57" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>50</v>
+      </c>
+      <c r="O58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B83" s="1"/>
+      <c r="O83" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:W7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Laporan Hari ke 6
</commit_message>
<xml_diff>
--- a/BACKLOG TKPPL.xlsx
+++ b/BACKLOG TKPPL.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\presentasi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7155" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7152" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Scrummaster" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="94">
   <si>
     <t>Penjelasan Tahapan Persiapan dan Sebelum memulai Proyek dengan Trello.</t>
   </si>
@@ -246,6 +246,72 @@
   </si>
   <si>
     <t>Ket : Untuk Penjelasan secara Umum : Elemen pada Dota2 (Game Mode, Aktor, Item) yang harusnya digeser ke Done oleh Javentira Lienata digantikan oleh ScrumMaster Sprint 1 (William Limianto) karena berhalangan.</t>
+  </si>
+  <si>
+    <t>7. Penjelasan secara Umum : Game Mode Dota2 (Penja</t>
+  </si>
+  <si>
+    <t>8. Penjelasan secara Umum : "Aktor" yang ada pada Dota2(Penjelasan untuk Creeps, Neutral Creeps, Tower, Ancient,Hero)</t>
+  </si>
+  <si>
+    <t>9. Role : Disabler</t>
+  </si>
+  <si>
+    <t>10. Role : Lane Support</t>
+  </si>
+  <si>
+    <t>11. Warding : Manfaat Warding.</t>
+  </si>
+  <si>
+    <t>12. Hero Guide Sniper : Item Build (Early, Mid, Late)</t>
+  </si>
+  <si>
+    <t>1. Penjelasan secara Umum : Effect Item pada Dota2 (Jenis dan Penjelasan, Beberapa Contoh)</t>
+  </si>
+  <si>
+    <t>2. Penjelasan secara Umum : Aturan Bermain Dota2</t>
+  </si>
+  <si>
+    <t>3. Penjelasan secara Umum : Manfaat Bermain Dota2</t>
+  </si>
+  <si>
+    <t>4. Role : Initiator</t>
+  </si>
+  <si>
+    <t>5. Role : Jungler</t>
+  </si>
+  <si>
+    <t>6. Role : Support</t>
+  </si>
+  <si>
+    <t>7. Role : Durable</t>
+  </si>
+  <si>
+    <t>8. Role : Nuker</t>
+  </si>
+  <si>
+    <t>9. Role : Pusher</t>
+  </si>
+  <si>
+    <t>10. Role : Escape</t>
+  </si>
+  <si>
+    <t>11. Warding : Jenis-Jenis Strategi Warding</t>
+  </si>
+  <si>
+    <t>12. Warding : Pembagian Ward (Penjelasan untuk Observer &amp; Sentry)</t>
+  </si>
+  <si>
+    <t>13. Warding : Lokasi Ideal untuk Warding</t>
+  </si>
+  <si>
+    <t>14. Hero Guide Sniper : Strategy (Early, Mid, Late)</t>
+  </si>
+  <si>
+    <t>15. Hero Guide Sniper : Best "Friends"</t>
+  </si>
+  <si>
+    <t>16. Hero Guide Sniper : Worst "Enemies"</t>
   </si>
 </sst>
 </file>
@@ -405,6 +471,55 @@
         <a:xfrm>
           <a:off x="666752" y="2690809"/>
           <a:ext cx="12923809" cy="6295238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>182498</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="2125980"/>
+          <a:ext cx="12161520" cy="5851778"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -683,9 +798,9 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
@@ -711,7 +826,7 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -735,7 +850,7 @@
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -759,7 +874,7 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -783,7 +898,7 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -807,7 +922,7 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -831,7 +946,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>16</v>
       </c>
@@ -842,7 +957,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>19</v>
       </c>
@@ -853,7 +968,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>21</v>
       </c>
@@ -864,7 +979,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>23</v>
       </c>
@@ -875,7 +990,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>25</v>
       </c>
@@ -899,13 +1014,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W83"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B52" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -931,7 +1046,7 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -955,7 +1070,7 @@
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -979,7 +1094,7 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1003,7 +1118,7 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1027,7 +1142,7 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1051,7 +1166,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="10" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:23" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1061,7 +1176,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B52" s="1" t="s">
         <v>1</v>
       </c>
@@ -1069,147 +1184,147 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B83" s="1"/>
       <c r="O83" s="1"/>
     </row>
@@ -1227,11 +1342,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView topLeftCell="A41" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AC16" sqref="AC16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>44</v>
       </c>
@@ -1257,7 +1374,7 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1281,7 +1398,7 @@
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1305,7 +1422,7 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1329,7 +1446,7 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1353,7 +1470,7 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1377,7 +1494,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="10" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:23" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1387,12 +1504,12 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B49" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B52" s="1" t="s">
         <v>1</v>
       </c>
@@ -1400,7 +1517,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>45</v>
       </c>
@@ -1408,7 +1525,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>46</v>
       </c>
@@ -1416,7 +1533,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>47</v>
       </c>
@@ -1424,7 +1541,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>48</v>
       </c>
@@ -1432,7 +1549,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>49</v>
       </c>
@@ -1440,7 +1557,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>50</v>
       </c>
@@ -1448,87 +1565,87 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B83" s="1"/>
       <c r="O83" s="1"/>
     </row>
@@ -1544,13 +1661,304 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:W83"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="M57" sqref="M57"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+    </row>
+    <row r="10" spans="2:23" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>78</v>
+      </c>
+      <c r="O46" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>79</v>
+      </c>
+      <c r="O47" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>80</v>
+      </c>
+      <c r="O48" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>81</v>
+      </c>
+      <c r="O49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>82</v>
+      </c>
+      <c r="O50" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>83</v>
+      </c>
+      <c r="O51" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>84</v>
+      </c>
+      <c r="O52" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>85</v>
+      </c>
+      <c r="O53" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>86</v>
+      </c>
+      <c r="O54" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>87</v>
+      </c>
+      <c r="O55" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>88</v>
+      </c>
+      <c r="O56" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>89</v>
+      </c>
+      <c r="O57" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="60" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="83" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B83" s="1"/>
+      <c r="O83" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:W7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1560,7 +1968,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1572,7 +1980,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1584,7 +1992,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Laporan Burndown Chart dan Log Book Hari ke-7.
</commit_message>
<xml_diff>
--- a/BACKLOG TKPPL.xlsx
+++ b/BACKLOG TKPPL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\presentasi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="95">
   <si>
     <t>Penjelasan Tahapan Persiapan dan Sebelum memulai Proyek dengan Trello.</t>
   </si>
@@ -312,6 +312,9 @@
   </si>
   <si>
     <t>16. Hero Guide Sniper : Worst "Enemies"</t>
+  </si>
+  <si>
+    <t>Penjelasan Hasil Sprint Kedua dengan Trello.</t>
   </si>
 </sst>
 </file>
@@ -1663,15 +1666,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>

</xml_diff>

<commit_message>
Laporan Burndown Chart, Log Book Hari ke 9.
</commit_message>
<xml_diff>
--- a/BACKLOG TKPPL.xlsx
+++ b/BACKLOG TKPPL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7152" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7152" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Scrummaster" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="112">
   <si>
     <t>Penjelasan Tahapan Persiapan dan Sebelum memulai Proyek dengan Trello.</t>
   </si>
@@ -315,6 +315,57 @@
   </si>
   <si>
     <t>Penjelasan Hasil Sprint Kedua dengan Trello.</t>
+  </si>
+  <si>
+    <t>1. Penjelasan secara Umum : Aturan Bermain Dota2</t>
+  </si>
+  <si>
+    <t>2. Penjelasan secara Umum : Manfaat Bermain Dota2</t>
+  </si>
+  <si>
+    <t>3. Role : Support</t>
+  </si>
+  <si>
+    <t>4. Role : Durable</t>
+  </si>
+  <si>
+    <t>5. Role : Nuker</t>
+  </si>
+  <si>
+    <t>6. Role : Pusher</t>
+  </si>
+  <si>
+    <t>7. Role : Escape</t>
+  </si>
+  <si>
+    <t>8. Warding : Jenis-Jenis Strategi Warding</t>
+  </si>
+  <si>
+    <t>9. Warding : Lokasi Ideal untuk Warding</t>
+  </si>
+  <si>
+    <t>10. Hero Guide Sniper : Best "Friends"</t>
+  </si>
+  <si>
+    <t>11. Hero Guide Sniper : Worst "Enemies"</t>
+  </si>
+  <si>
+    <t>13. Penjelasan secara Umum : Effect Item pada Dota2 (Jenis dan Penjelasan, Beberapa Contoh)</t>
+  </si>
+  <si>
+    <t>14. Role : Initiator</t>
+  </si>
+  <si>
+    <t>15. Role : Jungler</t>
+  </si>
+  <si>
+    <t>16. Warding : Pembagian Ward (Penjelasan untuk Observer &amp; Sentry)</t>
+  </si>
+  <si>
+    <t>17. Hero Guide Sniper : Strategy (Early, Mid, Late)</t>
+  </si>
+  <si>
+    <t>Penjelasan Hasil Sprint Ketiga dengan Trello.</t>
   </si>
 </sst>
 </file>
@@ -523,6 +574,55 @@
         <a:xfrm>
           <a:off x="609600" y="2125980"/>
           <a:ext cx="12161520" cy="5851778"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>599886</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="624840" y="2133600"/>
+          <a:ext cx="12167046" cy="5814060"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1346,7 +1446,7 @@
   <dimension ref="B2:W83"/>
   <sheetViews>
     <sheetView topLeftCell="A41" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AC16" sqref="AC16"/>
+      <selection activeCell="N62" sqref="N62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1666,7 +1766,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K55" sqref="K55"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1965,13 +2067,306 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:W83"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+    </row>
+    <row r="10" spans="2:23" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>95</v>
+      </c>
+      <c r="O46" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>96</v>
+      </c>
+      <c r="O47" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>97</v>
+      </c>
+      <c r="O48" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>98</v>
+      </c>
+      <c r="O49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>99</v>
+      </c>
+      <c r="O50" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>100</v>
+      </c>
+      <c r="O51" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>101</v>
+      </c>
+      <c r="O52" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>102</v>
+      </c>
+      <c r="O53" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>103</v>
+      </c>
+      <c r="O54" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>104</v>
+      </c>
+      <c r="O55" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>105</v>
+      </c>
+      <c r="O56" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="O57" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="O58" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="59" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="O59" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="60" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="O60" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="O61" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="62" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="O62" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="83" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B83" s="1"/>
+      <c r="O83" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:W7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
logbook,burndown hari 12 + backlog sprint 4
</commit_message>
<xml_diff>
--- a/BACKLOG TKPPL.xlsx
+++ b/BACKLOG TKPPL.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\presentasi\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7152" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7155" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Scrummaster" sheetId="6" r:id="rId1"/>
@@ -20,9 +15,9 @@
     <sheet name="Sprint 4" sheetId="4" r:id="rId6"/>
     <sheet name="Sprint 5" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -30,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="139">
   <si>
     <t>Penjelasan Tahapan Persiapan dan Sebelum memulai Proyek dengan Trello.</t>
   </si>
@@ -366,13 +361,94 @@
   </si>
   <si>
     <t>Penjelasan Hasil Sprint Ketiga dengan Trello.</t>
+  </si>
+  <si>
+    <t>Penjelasan Hasil Sprint Keempat dengan Trello.</t>
+  </si>
+  <si>
+    <t>1. Penjelasan secara Umum : Manfaat Bermain Dota2</t>
+  </si>
+  <si>
+    <t>2. Role : Pusher</t>
+  </si>
+  <si>
+    <t>3. Role : Escape</t>
+  </si>
+  <si>
+    <t>4. Warding : Lokasi Ideal untuk Warding</t>
+  </si>
+  <si>
+    <t>5. Hero Guide Sniper : Worst "Enemies"</t>
+  </si>
+  <si>
+    <t>2. Role : Support</t>
+  </si>
+  <si>
+    <t>3. Role : Durable</t>
+  </si>
+  <si>
+    <t>4. Role : Nuker</t>
+  </si>
+  <si>
+    <t>5. Warding : Jenis-Jenis Strategi Warding</t>
+  </si>
+  <si>
+    <t>6. Hero Guide Sniper : Best "Friends"</t>
+  </si>
+  <si>
+    <t>7. Penjelasan secara Umum : Apa itu Dota2</t>
+  </si>
+  <si>
+    <t>8. Penjelasan secara Umum : Elemen pada Dota2 (Game Mode, Aktor, Item)</t>
+  </si>
+  <si>
+    <t>9. Edit Fungsionalitas dan Tampilan Bespoke</t>
+  </si>
+  <si>
+    <t>10. Role : Carry</t>
+  </si>
+  <si>
+    <t>11. Warding : Penjelasan</t>
+  </si>
+  <si>
+    <t>12. Hero Guide Sniper : Penjelasan Singkat (Tipe, Skills)</t>
+  </si>
+  <si>
+    <t>13. Penjelasan secara Umum : Game Mode Dota2 (Penja</t>
+  </si>
+  <si>
+    <t>14. Penjelasan secara Umum : "Aktor" yang ada pada Dota2(Penjelasan untuk Creeps, Neutral Creeps, Tower, Ancient,Hero)</t>
+  </si>
+  <si>
+    <t>15. Role : Disabler</t>
+  </si>
+  <si>
+    <t>16. Role : Lane Support</t>
+  </si>
+  <si>
+    <t>17. Warding : Manfaat Warding.</t>
+  </si>
+  <si>
+    <t>18. Hero Guide Sniper : Item Build (Early, Mid, Late)</t>
+  </si>
+  <si>
+    <t>19. Penjelasan secara Umum : Effect Item pada Dota2 (Jenis dan Penjelasan, Beberapa Contoh)</t>
+  </si>
+  <si>
+    <t>20. Role : Initiator</t>
+  </si>
+  <si>
+    <t>21. Role : Jungler</t>
+  </si>
+  <si>
+    <t>23. Hero Guide Sniper : Strategy (Early, Mid, Late)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -562,7 +638,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -611,7 +687,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -627,6 +703,58 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>503463</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1026" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="612321" y="2013857"/>
+          <a:ext cx="11525249" cy="6454140"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -677,7 +805,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -712,7 +840,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -889,21 +1017,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:W13"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:23">
       <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
@@ -929,7 +1057,7 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:23">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -953,7 +1081,7 @@
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:23">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -977,7 +1105,7 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:23">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1001,7 +1129,7 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:23">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1025,7 +1153,7 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:23">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1049,7 +1177,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:23">
       <c r="C9" t="s">
         <v>16</v>
       </c>
@@ -1060,7 +1188,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:23">
       <c r="C10" t="s">
         <v>19</v>
       </c>
@@ -1071,7 +1199,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:23">
       <c r="C11" t="s">
         <v>21</v>
       </c>
@@ -1082,7 +1210,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:23">
       <c r="C12" t="s">
         <v>23</v>
       </c>
@@ -1093,7 +1221,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:23">
       <c r="C13" t="s">
         <v>25</v>
       </c>
@@ -1114,16 +1242,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:W83"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:23">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1149,7 +1277,7 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:23">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1173,7 +1301,7 @@
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:23">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1197,7 +1325,7 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:23">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1221,7 +1349,7 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:23">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1245,7 +1373,7 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:23">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1269,7 +1397,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="10" spans="2:23" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:23" ht="23.25">
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1279,7 +1407,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:15">
       <c r="B52" s="1" t="s">
         <v>1</v>
       </c>
@@ -1287,147 +1415,147 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:15">
       <c r="B53" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:15">
       <c r="B54" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:15">
       <c r="B55" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:15">
       <c r="B56" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:15">
       <c r="B57" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:15">
       <c r="B58" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:15">
       <c r="B59" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:15">
       <c r="B60" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:15">
       <c r="B61" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:15">
       <c r="B62" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:15">
       <c r="B63" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:15">
       <c r="B64" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:2">
       <c r="B65" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:2">
       <c r="B66" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2">
       <c r="B67" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2">
       <c r="B68" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:2">
       <c r="B69" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:2">
       <c r="B70" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:2">
       <c r="B71" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:2">
       <c r="B72" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:2">
       <c r="B73" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:2">
       <c r="B74" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:2">
       <c r="B75" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:2">
       <c r="B76" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:2">
       <c r="B77" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:2">
       <c r="B78" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:2">
       <c r="B79" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:2">
       <c r="B80" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:15">
       <c r="B83" s="1"/>
       <c r="O83" s="1"/>
     </row>
@@ -1442,16 +1570,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:W83"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="N62" sqref="N62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:23">
       <c r="B2" s="3" t="s">
         <v>44</v>
       </c>
@@ -1477,7 +1605,7 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:23">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1501,7 +1629,7 @@
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:23">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1525,7 +1653,7 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:23">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1549,7 +1677,7 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:23">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1573,7 +1701,7 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:23">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1597,7 +1725,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="10" spans="2:23" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:23" ht="23.25">
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1607,12 +1735,12 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:15">
       <c r="B49" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:15">
       <c r="B52" s="1" t="s">
         <v>1</v>
       </c>
@@ -1620,7 +1748,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:15">
       <c r="B53" t="s">
         <v>45</v>
       </c>
@@ -1628,7 +1756,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:15">
       <c r="B54" t="s">
         <v>46</v>
       </c>
@@ -1636,7 +1764,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:15">
       <c r="B55" t="s">
         <v>47</v>
       </c>
@@ -1644,7 +1772,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:15">
       <c r="B56" t="s">
         <v>48</v>
       </c>
@@ -1652,7 +1780,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:15">
       <c r="B57" t="s">
         <v>49</v>
       </c>
@@ -1660,7 +1788,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:15">
       <c r="B58" t="s">
         <v>50</v>
       </c>
@@ -1668,87 +1796,87 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:15">
       <c r="B59" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:15">
       <c r="B60" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:15">
       <c r="B61" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:15">
       <c r="B62" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:15">
       <c r="B63" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:15">
       <c r="B64" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:2">
       <c r="B65" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:2">
       <c r="B66" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2">
       <c r="B67" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2">
       <c r="B68" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:2">
       <c r="B69" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:2">
       <c r="B70" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:2">
       <c r="B71" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:2">
       <c r="B72" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:2">
       <c r="B73" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:2">
       <c r="B74" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:15">
       <c r="B83" s="1"/>
       <c r="O83" s="1"/>
     </row>
@@ -1763,16 +1891,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:W83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:23">
       <c r="B2" s="3" t="s">
         <v>94</v>
       </c>
@@ -1798,7 +1926,7 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:23">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1822,7 +1950,7 @@
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:23">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1846,7 +1974,7 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:23">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1870,7 +1998,7 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:23">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1894,7 +2022,7 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:23">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1918,7 +2046,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="10" spans="2:23" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:23" ht="23.25">
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1928,7 +2056,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:15">
       <c r="B45" s="1" t="s">
         <v>1</v>
       </c>
@@ -1936,7 +2064,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:15">
       <c r="B46" t="s">
         <v>78</v>
       </c>
@@ -1944,7 +2072,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:15">
       <c r="B47" t="s">
         <v>79</v>
       </c>
@@ -1952,7 +2080,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:15">
       <c r="B48" t="s">
         <v>80</v>
       </c>
@@ -1960,7 +2088,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:15">
       <c r="B49" t="s">
         <v>81</v>
       </c>
@@ -1968,7 +2096,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:15">
       <c r="B50" t="s">
         <v>82</v>
       </c>
@@ -1976,7 +2104,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:15">
       <c r="B51" t="s">
         <v>83</v>
       </c>
@@ -1984,7 +2112,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:15">
       <c r="B52" t="s">
         <v>84</v>
       </c>
@@ -1992,7 +2120,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:15">
       <c r="B53" t="s">
         <v>85</v>
       </c>
@@ -2000,7 +2128,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:15">
       <c r="B54" t="s">
         <v>86</v>
       </c>
@@ -2008,7 +2136,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:15">
       <c r="B55" t="s">
         <v>87</v>
       </c>
@@ -2016,7 +2144,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:15">
       <c r="B56" t="s">
         <v>88</v>
       </c>
@@ -2024,7 +2152,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:15">
       <c r="B57" t="s">
         <v>89</v>
       </c>
@@ -2032,27 +2160,27 @@
         <v>77</v>
       </c>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:15">
       <c r="B58" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:15">
       <c r="B59" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:15">
       <c r="B60" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:15">
       <c r="B61" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:15">
       <c r="B83" s="1"/>
       <c r="O83" s="1"/>
     </row>
@@ -2066,16 +2194,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:W83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:23">
       <c r="B2" s="3" t="s">
         <v>111</v>
       </c>
@@ -2101,7 +2229,7 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:23">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2125,7 +2253,7 @@
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:23">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -2149,7 +2277,7 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:23">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -2173,7 +2301,7 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:23">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -2197,7 +2325,7 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:23">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -2221,7 +2349,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="10" spans="2:23" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:23" ht="23.25">
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
@@ -2231,7 +2359,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:15">
       <c r="B45" s="1" t="s">
         <v>1</v>
       </c>
@@ -2239,7 +2367,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:15">
       <c r="B46" t="s">
         <v>95</v>
       </c>
@@ -2247,7 +2375,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:15">
       <c r="B47" t="s">
         <v>96</v>
       </c>
@@ -2255,7 +2383,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:15">
       <c r="B48" t="s">
         <v>97</v>
       </c>
@@ -2263,7 +2391,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:15">
       <c r="B49" t="s">
         <v>98</v>
       </c>
@@ -2271,7 +2399,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:15">
       <c r="B50" t="s">
         <v>99</v>
       </c>
@@ -2279,7 +2407,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:15">
       <c r="B51" t="s">
         <v>100</v>
       </c>
@@ -2287,7 +2415,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:15">
       <c r="B52" t="s">
         <v>101</v>
       </c>
@@ -2295,7 +2423,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:15">
       <c r="B53" t="s">
         <v>102</v>
       </c>
@@ -2303,7 +2431,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:15">
       <c r="B54" t="s">
         <v>103</v>
       </c>
@@ -2311,7 +2439,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:15">
       <c r="B55" t="s">
         <v>104</v>
       </c>
@@ -2319,7 +2447,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:15">
       <c r="B56" t="s">
         <v>105</v>
       </c>
@@ -2327,37 +2455,37 @@
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:15">
       <c r="O57" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:15">
       <c r="O58" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:15">
       <c r="O59" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:15">
       <c r="O60" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:15">
       <c r="O61" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:15">
       <c r="O62" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:15">
       <c r="B83" s="1"/>
       <c r="O83" s="1"/>
     </row>
@@ -2371,24 +2499,329 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:W83"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="2:23">
+      <c r="B2" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+    </row>
+    <row r="3" spans="2:23">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+    </row>
+    <row r="4" spans="2:23">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+    </row>
+    <row r="5" spans="2:23">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+    </row>
+    <row r="6" spans="2:23">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+    </row>
+    <row r="7" spans="2:23">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+    </row>
+    <row r="10" spans="2:23" ht="23.25">
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="45" spans="2:15">
+      <c r="B45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15">
+      <c r="B46" t="s">
+        <v>113</v>
+      </c>
+      <c r="O46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15">
+      <c r="B47" t="s">
+        <v>114</v>
+      </c>
+      <c r="O47" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15">
+      <c r="B48" t="s">
+        <v>115</v>
+      </c>
+      <c r="O48" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15">
+      <c r="B49" t="s">
+        <v>116</v>
+      </c>
+      <c r="O49" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15">
+      <c r="B50" t="s">
+        <v>117</v>
+      </c>
+      <c r="O50" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="51" spans="2:15">
+      <c r="O51" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="2:15">
+      <c r="O52" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="2:15">
+      <c r="O53" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15">
+      <c r="O54" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="2:15">
+      <c r="O55" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15">
+      <c r="O56" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="57" spans="2:15">
+      <c r="O57" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="58" spans="2:15">
+      <c r="O58" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="59" spans="2:15">
+      <c r="O59" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="60" spans="2:15">
+      <c r="O60" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="61" spans="2:15">
+      <c r="O61" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="2:15">
+      <c r="O62" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="63" spans="2:15">
+      <c r="O63" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="64" spans="2:15">
+      <c r="O64" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="65" spans="15:15">
+      <c r="O65" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="66" spans="15:15">
+      <c r="O66" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="67" spans="15:15">
+      <c r="O67" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="68" spans="15:15">
+      <c r="O68" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="83" spans="2:15">
+      <c r="B83" s="1"/>
+      <c r="O83" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:W7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update benefit of playing dota 2
</commit_message>
<xml_diff>
--- a/BACKLOG TKPPL.xlsx
+++ b/BACKLOG TKPPL.xlsx
@@ -623,7 +623,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -672,7 +672,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1002,7 +1002,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1230,8 +1230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:W83"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J61" sqref="J61"/>
+    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53:D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2488,7 +2488,7 @@
   <dimension ref="B2:W83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Tambah Laporan Log Book dan Burndown Chart hari ke-13.
</commit_message>
<xml_diff>
--- a/BACKLOG TKPPL.xlsx
+++ b/BACKLOG TKPPL.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\presentasi\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7155" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7155" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Scrummaster" sheetId="6" r:id="rId1"/>
@@ -15,9 +20,9 @@
     <sheet name="Sprint 4" sheetId="4" r:id="rId6"/>
     <sheet name="Sprint 5" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -432,8 +437,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -623,7 +628,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -672,7 +677,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1002,21 +1007,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W13"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:23">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
@@ -1042,7 +1047,7 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="3" spans="2:23">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1066,7 +1071,7 @@
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="2:23">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1090,7 +1095,7 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="2:23">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1114,7 +1119,7 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="2:23">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1138,7 +1143,7 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="2:23">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1162,7 +1167,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="9" spans="2:23">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>16</v>
       </c>
@@ -1173,7 +1178,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:23">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>19</v>
       </c>
@@ -1184,7 +1189,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:23">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>21</v>
       </c>
@@ -1195,7 +1200,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:23">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>23</v>
       </c>
@@ -1206,7 +1211,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:23">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>25</v>
       </c>
@@ -1227,16 +1232,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W83"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53:D80"/>
-    </sheetView>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:23">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1262,7 +1265,7 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="3" spans="2:23">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1286,7 +1289,7 @@
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="2:23">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1310,7 +1313,7 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="2:23">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1334,7 +1337,7 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="2:23">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1358,7 +1361,7 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="2:23">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1382,7 +1385,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="10" spans="2:23" ht="23.25">
+    <row r="10" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1392,7 +1395,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="52" spans="2:15">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>1</v>
       </c>
@@ -1400,147 +1403,147 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="2:15">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="2:15">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="2:15">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="2:15">
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="2:15">
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="2:15">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="2:15">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="2:15">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="2:15">
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="2:15">
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="2:15">
+    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="2:15">
+    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="2:2">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="2:2">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="2:2">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="2:2">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="2:2">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="2:2">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="2:2">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="2:2">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="2:2">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="2:2">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="2:2">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="76" spans="2:2">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="77" spans="2:2">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="78" spans="2:2">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="79" spans="2:2">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="80" spans="2:2">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="83" spans="2:15">
+    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
       <c r="O83" s="1"/>
     </row>
@@ -1555,16 +1558,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W83"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N62" sqref="N62"/>
-    </sheetView>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:23">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>44</v>
       </c>
@@ -1590,7 +1591,7 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="3" spans="2:23">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1614,7 +1615,7 @@
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="2:23">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1638,7 +1639,7 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="2:23">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1662,7 +1663,7 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="2:23">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1686,7 +1687,7 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="2:23">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1710,7 +1711,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="10" spans="2:23" ht="23.25">
+    <row r="10" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1720,12 +1721,12 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="49" spans="2:15">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="2:15">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>1</v>
       </c>
@@ -1733,7 +1734,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="2:15">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>45</v>
       </c>
@@ -1741,7 +1742,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="2:15">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>46</v>
       </c>
@@ -1749,7 +1750,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="2:15">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>47</v>
       </c>
@@ -1757,7 +1758,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="2:15">
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>48</v>
       </c>
@@ -1765,7 +1766,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="2:15">
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>49</v>
       </c>
@@ -1773,7 +1774,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="2:15">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>50</v>
       </c>
@@ -1781,87 +1782,87 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="2:15">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="2:15">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="61" spans="2:15">
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="2:15">
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="2:15">
+    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="2:15">
+    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="65" spans="2:2">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="66" spans="2:2">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="67" spans="2:2">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="68" spans="2:2">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="2:2">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="70" spans="2:2">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="71" spans="2:2">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="72" spans="2:2">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="73" spans="2:2">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="2:2">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="83" spans="2:15">
+    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
       <c r="O83" s="1"/>
     </row>
@@ -1876,16 +1877,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W83"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K55" sqref="K55"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:23">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>94</v>
       </c>
@@ -1911,7 +1910,7 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="3" spans="2:23">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1935,7 +1934,7 @@
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="2:23">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1959,7 +1958,7 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="2:23">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1983,7 +1982,7 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="2:23">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -2007,7 +2006,7 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="2:23">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -2031,7 +2030,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="10" spans="2:23" ht="23.25">
+    <row r="10" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
@@ -2041,7 +2040,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="45" spans="2:15">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>1</v>
       </c>
@@ -2049,7 +2048,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="2:15">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>78</v>
       </c>
@@ -2057,7 +2056,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="2:15">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>79</v>
       </c>
@@ -2065,7 +2064,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="2:15">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>80</v>
       </c>
@@ -2073,7 +2072,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="2:15">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>81</v>
       </c>
@@ -2081,7 +2080,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="2:15">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>82</v>
       </c>
@@ -2089,7 +2088,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="2:15">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>83</v>
       </c>
@@ -2097,7 +2096,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="2:15">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>84</v>
       </c>
@@ -2105,7 +2104,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="2:15">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>85</v>
       </c>
@@ -2113,7 +2112,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="2:15">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>86</v>
       </c>
@@ -2121,7 +2120,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="2:15">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>87</v>
       </c>
@@ -2129,7 +2128,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="2:15">
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>88</v>
       </c>
@@ -2137,7 +2136,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="2:15">
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>89</v>
       </c>
@@ -2145,27 +2144,27 @@
         <v>77</v>
       </c>
     </row>
-    <row r="58" spans="2:15">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="2:15">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="60" spans="2:15">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="61" spans="2:15">
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="83" spans="2:15">
+    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
       <c r="O83" s="1"/>
     </row>
@@ -2179,16 +2178,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W83"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:23">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>111</v>
       </c>
@@ -2214,7 +2211,7 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="3" spans="2:23">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2238,7 +2235,7 @@
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="2:23">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -2262,7 +2259,7 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="2:23">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -2286,7 +2283,7 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="2:23">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -2310,7 +2307,7 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="2:23">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -2334,7 +2331,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="10" spans="2:23" ht="23.25">
+    <row r="10" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
@@ -2344,7 +2341,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="45" spans="2:15">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>1</v>
       </c>
@@ -2352,7 +2349,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="2:15">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>95</v>
       </c>
@@ -2360,7 +2357,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="2:15">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>96</v>
       </c>
@@ -2368,7 +2365,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="2:15">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>97</v>
       </c>
@@ -2376,7 +2373,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="2:15">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>98</v>
       </c>
@@ -2384,7 +2381,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="2:15">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>99</v>
       </c>
@@ -2392,7 +2389,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="2:15">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>100</v>
       </c>
@@ -2400,7 +2397,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="52" spans="2:15">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>101</v>
       </c>
@@ -2408,7 +2405,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="2:15">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>102</v>
       </c>
@@ -2416,7 +2413,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="54" spans="2:15">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>103</v>
       </c>
@@ -2424,7 +2421,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="2:15">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>104</v>
       </c>
@@ -2432,7 +2429,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="2:15">
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>105</v>
       </c>
@@ -2440,37 +2437,37 @@
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="2:15">
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O57" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="58" spans="2:15">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O58" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="59" spans="2:15">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O59" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="60" spans="2:15">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O60" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="61" spans="2:15">
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O61" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="62" spans="2:15">
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O62" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="83" spans="2:15">
+    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
       <c r="O83" s="1"/>
     </row>
@@ -2484,16 +2481,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:23">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>112</v>
       </c>
@@ -2519,7 +2514,7 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="3" spans="2:23">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2543,7 +2538,7 @@
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="2:23">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -2567,7 +2562,7 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="2:23">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -2591,7 +2586,7 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="2:23">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -2615,7 +2610,7 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="2:23">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -2639,7 +2634,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="10" spans="2:23" ht="23.25">
+    <row r="10" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
@@ -2649,7 +2644,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="45" spans="2:15">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>1</v>
       </c>
@@ -2657,7 +2652,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="2:15">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>113</v>
       </c>
@@ -2665,7 +2660,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="2:15">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>114</v>
       </c>
@@ -2673,7 +2668,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="48" spans="2:15">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>115</v>
       </c>
@@ -2681,7 +2676,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="49" spans="2:15">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>116</v>
       </c>
@@ -2689,7 +2684,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="50" spans="2:15">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>117</v>
       </c>
@@ -2697,97 +2692,97 @@
         <v>121</v>
       </c>
     </row>
-    <row r="51" spans="2:15">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O51" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="2:15">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O52" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="2:15">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O53" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="54" spans="2:15">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O54" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="2:15">
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O55" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="2:15">
+    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O56" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="57" spans="2:15">
+    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O57" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="2:15">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O58" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="2:15">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O59" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="2:15">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O60" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="2:15">
+    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O61" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="2:15">
+    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O62" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="63" spans="2:15">
+    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O63" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="64" spans="2:15">
+    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O64" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="65" spans="15:15">
+    <row r="65" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O65" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="66" spans="15:15">
+    <row r="66" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O66" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="15:15">
+    <row r="67" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O67" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="15:15">
+    <row r="68" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O68" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="83" spans="2:15">
+    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
       <c r="O83" s="1"/>
     </row>
@@ -2801,12 +2796,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Tambah Laporan Log Book, Burndown Chart, dan Backlog Hari ke-14.
</commit_message>
<xml_diff>
--- a/BACKLOG TKPPL.xlsx
+++ b/BACKLOG TKPPL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7155" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="Scrummaster" sheetId="6" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sprint 2" sheetId="2" r:id="rId4"/>
     <sheet name="Sprint 3" sheetId="3" r:id="rId5"/>
     <sheet name="Sprint 4" sheetId="4" r:id="rId6"/>
-    <sheet name="Sprint 5" sheetId="7" r:id="rId7"/>
+    <sheet name="Sprint 5" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="135">
   <si>
     <t>Penjelasan Tahapan Persiapan dan Sebelum memulai Proyek dengan Trello.</t>
   </si>
@@ -432,6 +432,9 @@
   </si>
   <si>
     <t>23. Hero Guide Sniper : Best "Friends"</t>
+  </si>
+  <si>
+    <t>Penjelasan Hasil Sprint Kelima dengan Trello.</t>
   </si>
 </sst>
 </file>
@@ -752,6 +755,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>122209</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>8738</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="2009775"/>
+          <a:ext cx="12923809" cy="6295238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1017,7 +1063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W13"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2484,7 +2530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -2797,12 +2843,325 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:W83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+    </row>
+    <row r="10" spans="2:23" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="O46" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="O47" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="O48" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O49" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O50" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O51" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O52" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O53" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O55" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O58" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O59" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O62" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O63" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O64" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O65" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="66" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O66" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O67" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="68" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O68" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="69" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O69" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="70" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O70" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O71" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="72" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O72" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="73" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O73" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B83" s="1"/>
+      <c r="O83" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:W7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>